<commit_message>
Beginning of CSS practice
</commit_message>
<xml_diff>
--- a/Coding Bootcamp Schedule.xlsx
+++ b/Coding Bootcamp Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Desktop\WebDev Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF8EEBE-46E8-45C1-A2D8-BECFF4ED5B98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150D03A4-2677-4A2F-8868-CE74883A2AD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{297EB169-FCC9-4576-8CD7-D3A5F8629C68}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>57: What Matters in this Section</t>
+  </si>
+  <si>
+    <t>Coding Exercise 11: Checkerboard Exercise</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -691,6 +694,13 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <f>60+43</f>
+        <v>103</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D13" s="7" t="s">
@@ -707,7 +717,7 @@
       </c>
       <c r="E14" s="4">
         <f>SUM(E3:E6)</f>
-        <v>189</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -722,7 +732,10 @@
       <c r="D16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4">
+        <f>SUM(E6:E8)</f>
+        <v>103</v>
+      </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D17" s="8" t="s">
@@ -748,7 +761,7 @@
       </c>
       <c r="E20" s="6">
         <f>SUM(E13:E19)</f>
-        <v>301</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.45">
@@ -757,7 +770,7 @@
       </c>
       <c r="E21" s="5">
         <f>E20/60/63</f>
-        <v>7.9629629629629634E-2</v>
+        <v>0.13412698412698412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More CSS and File Reorganization
</commit_message>
<xml_diff>
--- a/Coding Bootcamp Schedule.xlsx
+++ b/Coding Bootcamp Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Desktop\WebDev Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150D03A4-2677-4A2F-8868-CE74883A2AD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9105FE06-8645-442F-B77D-40C711776793}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{297EB169-FCC9-4576-8CD7-D3A5F8629C68}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Coding Exercise 11: Checkerboard Exercise</t>
+  </si>
+  <si>
+    <t>76: Pseudo Elements</t>
   </si>
 </sst>
 </file>
@@ -582,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4091C950-023E-4CEE-ADD0-7B11E9C695F9}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -702,75 +705,100 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D13" s="7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44323</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <f>27+68</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E14" s="3">
         <f>E2</f>
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="4">
-        <f>SUM(E3:E6)</f>
-        <v>292</v>
-      </c>
-    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D15" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="4">
-        <v>0</v>
+        <f>SUM(E3:E5)</f>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D16" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="4">
-        <f>SUM(E6:E8)</f>
-        <v>103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="E17" s="4">
+        <f>SUM(E6:E8)</f>
+        <v>198</v>
+      </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.45">
+      <c r="D20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="D20" s="9" t="s">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.45">
+      <c r="D21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="6">
-        <f>SUM(E13:E19)</f>
-        <v>507</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="6">
+        <f>SUM(E14:E20)</f>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.45">
+      <c r="D22" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="5">
-        <f>E20/60/63</f>
-        <v>0.13412698412698412</v>
+      <c r="E22" s="5">
+        <f>E21/60/63</f>
+        <v>0.13201058201058199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>